<commit_message>
change logs: 1. Add detail to notebook 2. Support xlwings 0.21.0 and RDP alpha 7
</commit_message>
<xml_diff>
--- a/notebook/part2_rdp_intel_vs_amd.xlsx
+++ b/notebook/part2_rdp_intel_vs_amd.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\drive_d\Project\Code\xlwings_project\notebook\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{85E7C024-C1E7-4C29-91DB-C330744C8520}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A86C1A8D-EF25-408B-B336-0F98163556EC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="25440" windowHeight="15540" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-23148" yWindow="-420" windowWidth="23256" windowHeight="12720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Intel vs AMD Daiy Price" sheetId="4" r:id="rId1"/>
@@ -224,7 +224,7 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>11</xdr:col>
-      <xdr:colOff>141734</xdr:colOff>
+      <xdr:colOff>145544</xdr:colOff>
       <xdr:row>37</xdr:row>
       <xdr:rowOff>118494</xdr:rowOff>
     </xdr:to>
@@ -233,7 +233,7 @@
         <xdr:cNvPr id="3" name="Picture 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{50946877-5ECD-42D0-B9E2-950276AC4A87}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{EF446989-54B6-414D-ACBA-5DAAF6A17E3A}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -256,7 +256,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="0" y="3505201"/>
-          <a:ext cx="7323584" cy="3737993"/>
+          <a:ext cx="7327394" cy="3737993"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -267,14 +267,14 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>13</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>605790</xdr:colOff>
       <xdr:row>18</xdr:row>
       <xdr:rowOff>1</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>24</xdr:col>
-      <xdr:colOff>141734</xdr:colOff>
+      <xdr:colOff>143639</xdr:colOff>
       <xdr:row>37</xdr:row>
       <xdr:rowOff>118494</xdr:rowOff>
     </xdr:to>
@@ -283,7 +283,7 @@
         <xdr:cNvPr id="5" name="Picture 4">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{DA78ACD8-0DD5-41C9-9164-DC9A33FC4F34}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D54B9FC8-6803-4F02-A0B1-BC55A93FB519}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -306,7 +306,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="8401050" y="3505201"/>
-          <a:ext cx="7323584" cy="3737993"/>
+          <a:ext cx="7325489" cy="3737993"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -329,7 +329,7 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>12</xdr:col>
-      <xdr:colOff>5614</xdr:colOff>
+      <xdr:colOff>3709</xdr:colOff>
       <xdr:row>21</xdr:row>
       <xdr:rowOff>40906</xdr:rowOff>
     </xdr:to>
@@ -338,7 +338,7 @@
         <xdr:cNvPr id="3" name="Picture 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A60F1750-3D65-4668-A623-8B7A16FEFB41}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2FC1DE37-F532-495B-8F52-21DEFFADDB9A}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -361,7 +361,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="1" y="457200"/>
-          <a:ext cx="7320813" cy="3660406"/>
+          <a:ext cx="7318908" cy="3660406"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -387,13 +387,13 @@
   </autoFilter>
   <tableColumns count="8">
     <tableColumn id="1" xr3:uid="{84126F28-5BA5-43DA-87E1-D851FF53831B}" name="Date"/>
-    <tableColumn id="2" xr3:uid="{1B759AEB-2724-4D7D-A1A3-C3CCBCE5D045}" name="BID"/>
-    <tableColumn id="3" xr3:uid="{823CA538-2255-42FC-AAC4-53CEB33488F8}" name="ASK"/>
-    <tableColumn id="4" xr3:uid="{102AD010-C86C-45FD-B3ED-71116A93BF12}" name="OPEN_PRC"/>
-    <tableColumn id="5" xr3:uid="{1AA0A6F5-3C0F-45DB-8200-BE054321EFBC}" name="HIGH_1"/>
-    <tableColumn id="6" xr3:uid="{A88DEFEB-BB3A-4BCA-B9B9-CD4F9EF270FB}" name="LOW_1"/>
-    <tableColumn id="7" xr3:uid="{4ED05AE9-0705-4FE7-BC5B-98FC1457860D}" name="TRDPRC_1"/>
-    <tableColumn id="8" xr3:uid="{F44E82BE-B936-48E1-A820-DE260FB305BA}" name="BLKVOLUM"/>
+    <tableColumn id="2" xr3:uid="{4DDB8E2E-2426-464A-9103-7AFCC22406D5}" name="BID"/>
+    <tableColumn id="3" xr3:uid="{811D0C93-38D4-449B-B853-A222C92603A0}" name="ASK"/>
+    <tableColumn id="4" xr3:uid="{FEA74A4D-C0C4-499C-817B-5F503343491E}" name="OPEN_PRC"/>
+    <tableColumn id="5" xr3:uid="{9F11C1DE-3CD6-45C8-892D-CB3DEE33D4B4}" name="HIGH_1"/>
+    <tableColumn id="6" xr3:uid="{925DE222-5C59-4614-A170-D14E344DBE55}" name="LOW_1"/>
+    <tableColumn id="7" xr3:uid="{709193ED-1F36-45A8-A0DF-C1BAEACB8B54}" name="TRDPRC_1"/>
+    <tableColumn id="8" xr3:uid="{B939FCC6-A8A2-48EA-8C27-BB2D81D30E3B}" name="BLKVOLUM"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium14" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -413,13 +413,13 @@
   </autoFilter>
   <tableColumns count="8">
     <tableColumn id="1" xr3:uid="{A67C05C2-23BE-499F-A773-B002393BCD63}" name="Date"/>
-    <tableColumn id="2" xr3:uid="{3B1E6387-F22E-4BC5-95C8-A3746FD04BDF}" name="BID"/>
-    <tableColumn id="3" xr3:uid="{499C668B-7150-4D1C-90D6-7421EDF22F98}" name="ASK"/>
-    <tableColumn id="4" xr3:uid="{3407628B-F4F7-494D-AF78-B5F5FF3F285E}" name="OPEN_PRC"/>
-    <tableColumn id="5" xr3:uid="{8B914C9E-23D0-4BCF-BE26-923B4AFE8E88}" name="HIGH_1"/>
-    <tableColumn id="6" xr3:uid="{D8ACC2EE-D2F1-405B-8E45-39D01A832A50}" name="LOW_1"/>
-    <tableColumn id="7" xr3:uid="{5F3CC3AF-A9FE-4B9F-9BD0-9E051A2FEDB0}" name="TRDPRC_1"/>
-    <tableColumn id="8" xr3:uid="{D0780F4C-A818-409A-AD44-740BD847CC26}" name="BLKVOLUM"/>
+    <tableColumn id="2" xr3:uid="{736B5D87-1F0F-4EC7-BA3B-992B607E9328}" name="BID"/>
+    <tableColumn id="3" xr3:uid="{5028BFDC-A9AB-423C-B31D-9F55FA6E714A}" name="ASK"/>
+    <tableColumn id="4" xr3:uid="{2EBDE992-A77B-4AC1-89DE-6F16C810F222}" name="OPEN_PRC"/>
+    <tableColumn id="5" xr3:uid="{68E6AABD-ED69-48D0-B832-ECFB8EDA571A}" name="HIGH_1"/>
+    <tableColumn id="6" xr3:uid="{8F24F082-860F-4740-A81B-9F07EDA05766}" name="LOW_1"/>
+    <tableColumn id="7" xr3:uid="{7086EC7C-3DB2-49B6-B84B-0CC34E72156B}" name="TRDPRC_1"/>
+    <tableColumn id="8" xr3:uid="{F9405C3E-AFE3-4052-8563-4F93B05A04C8}" name="BLKVOLUM"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium14" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -690,7 +690,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FB8FC013-95A6-4FF9-BDAB-F9F2B6095DAD}">
   <dimension ref="A1:U24"/>
   <sheetViews>
-    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="N3" sqref="N3:U17"/>
     </sheetView>
   </sheetViews>
@@ -1547,7 +1547,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{02D73A5B-02D3-46B4-9463-35316D3660EB}">
   <dimension ref="A1:N1"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="O7" sqref="O7"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
now support xlwings 0.21.3 and introudction to xlwings 0.21.4
</commit_message>
<xml_diff>
--- a/notebook/part2_rdp_intel_vs_amd.xlsx
+++ b/notebook/part2_rdp_intel_vs_amd.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\drive_d\Project\Code\xlwings_project\notebook\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C22E4357-E6A4-42AB-B915-80DC21DBBE6A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D46040D7-74F2-42B7-AAB9-E4BFADC49B3D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-1260" yWindow="1650" windowWidth="21390" windowHeight="11160" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView minimized="1" xWindow="3075" yWindow="3075" windowWidth="18900" windowHeight="11160" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Intel vs AMD Daily Price" sheetId="4" r:id="rId1"/>
@@ -220,20 +220,20 @@
       <xdr:col>0</xdr:col>
       <xdr:colOff>0</xdr:colOff>
       <xdr:row>18</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
+      <xdr:rowOff>1</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>11</xdr:col>
-      <xdr:colOff>152818</xdr:colOff>
+      <xdr:colOff>141734</xdr:colOff>
       <xdr:row>37</xdr:row>
-      <xdr:rowOff>157286</xdr:rowOff>
+      <xdr:rowOff>118494</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
         <xdr:cNvPr id="3" name="Picture 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{168B8A7B-A314-45EE-B466-492D769732A2}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A6645839-19C6-4434-AF7F-EEFE494BDD02}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -255,8 +255,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="0" y="3505200"/>
-          <a:ext cx="7334668" cy="3776786"/>
+          <a:off x="0" y="3505201"/>
+          <a:ext cx="7323584" cy="3737993"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -268,22 +268,22 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>13</xdr:col>
-      <xdr:colOff>1</xdr:colOff>
+      <xdr:colOff>0</xdr:colOff>
       <xdr:row>18</xdr:row>
       <xdr:rowOff>1</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>24</xdr:col>
-      <xdr:colOff>116796</xdr:colOff>
-      <xdr:row>38</xdr:row>
-      <xdr:rowOff>24976</xdr:rowOff>
+      <xdr:colOff>141734</xdr:colOff>
+      <xdr:row>37</xdr:row>
+      <xdr:rowOff>118494</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
         <xdr:cNvPr id="5" name="Picture 4">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6483FD23-32D1-4231-BE12-61444F87F949}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0094F4AC-C11E-47A3-87F9-418087454C18}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -305,8 +305,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="8401051" y="3505201"/>
-          <a:ext cx="7298645" cy="3834975"/>
+          <a:off x="8401050" y="3505201"/>
+          <a:ext cx="7323584" cy="3737993"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -338,7 +338,7 @@
         <xdr:cNvPr id="3" name="Picture 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{58304992-43EB-47E6-8792-DE159037C653}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{FE1E144B-1A78-4854-9752-6E9EFEBCCA4B}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -387,13 +387,13 @@
   </autoFilter>
   <tableColumns count="8">
     <tableColumn id="1" xr3:uid="{84126F28-5BA5-43DA-87E1-D851FF53831B}" name="Date"/>
-    <tableColumn id="2" xr3:uid="{74F6ABAD-E006-4A59-A98A-366BA4E12E7E}" name="BID"/>
-    <tableColumn id="3" xr3:uid="{A50E8F7D-E958-4103-BF0B-5C3D351D5C00}" name="ASK"/>
-    <tableColumn id="4" xr3:uid="{9BE0725D-45A2-45BE-A41E-FF0D87E299EA}" name="OPEN_PRC"/>
-    <tableColumn id="5" xr3:uid="{C0373BBB-3527-43A1-986D-16F8148A6FE2}" name="HIGH_1"/>
-    <tableColumn id="6" xr3:uid="{82757867-ED13-48A5-AC38-03DB2CB967A6}" name="LOW_1"/>
-    <tableColumn id="7" xr3:uid="{E57DA56E-7888-497A-8FBF-0DACAE184303}" name="TRDPRC_1"/>
-    <tableColumn id="8" xr3:uid="{309608F0-DEC0-447F-9D31-D281B6688846}" name="BLKVOLUM"/>
+    <tableColumn id="2" xr3:uid="{55A72642-1185-456E-946D-1172D91FF33E}" name="BID"/>
+    <tableColumn id="3" xr3:uid="{EED878D6-C8F3-4F72-9332-AF2FD1D48759}" name="ASK"/>
+    <tableColumn id="4" xr3:uid="{BC9FBA74-607B-4400-827A-B5E94C90B968}" name="OPEN_PRC"/>
+    <tableColumn id="5" xr3:uid="{1BD69382-422A-48BB-A09D-F29BA3C947F7}" name="HIGH_1"/>
+    <tableColumn id="6" xr3:uid="{6870A09C-7010-4C95-AFE7-EE60266B5B0A}" name="LOW_1"/>
+    <tableColumn id="7" xr3:uid="{30C8DD34-20F4-40CC-AF25-8F49C20D877C}" name="TRDPRC_1"/>
+    <tableColumn id="8" xr3:uid="{8C52FC65-209B-4252-83DE-3CFDF0AACB14}" name="BLKVOLUM"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium14" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -413,13 +413,13 @@
   </autoFilter>
   <tableColumns count="8">
     <tableColumn id="1" xr3:uid="{A67C05C2-23BE-499F-A773-B002393BCD63}" name="Date"/>
-    <tableColumn id="2" xr3:uid="{EDEE6140-09F8-47E6-ABC9-46554564C463}" name="BID"/>
-    <tableColumn id="3" xr3:uid="{96EA3098-D504-47FB-A910-6B025D518C14}" name="ASK"/>
-    <tableColumn id="4" xr3:uid="{B9E97F32-0C37-40E6-BCA1-FDE23677CA2C}" name="OPEN_PRC"/>
-    <tableColumn id="5" xr3:uid="{A43B7A30-248C-490E-B660-A635A185A959}" name="HIGH_1"/>
-    <tableColumn id="6" xr3:uid="{946AE44B-AFE8-4B93-8CFB-35A76F9E4554}" name="LOW_1"/>
-    <tableColumn id="7" xr3:uid="{1C2EA7DA-0062-4CDC-A739-8FC535253550}" name="TRDPRC_1"/>
-    <tableColumn id="8" xr3:uid="{1EC7CA39-BE32-4DAB-85E0-2D8FDF148D94}" name="BLKVOLUM"/>
+    <tableColumn id="2" xr3:uid="{8922C121-CCD8-49A6-A8AA-B0DFB6926B36}" name="BID"/>
+    <tableColumn id="3" xr3:uid="{3E61AE70-451D-42C7-80A9-3A4634BD0CED}" name="ASK"/>
+    <tableColumn id="4" xr3:uid="{1E62800E-183E-48D5-966E-11555EC968AC}" name="OPEN_PRC"/>
+    <tableColumn id="5" xr3:uid="{9291A001-515C-49EB-A243-A1E33E0ACF9A}" name="HIGH_1"/>
+    <tableColumn id="6" xr3:uid="{6B1DA8DC-6F25-48D5-9C95-814F829B41E3}" name="LOW_1"/>
+    <tableColumn id="7" xr3:uid="{6A4C1BB1-99A2-471B-948A-E344851C5CF1}" name="TRDPRC_1"/>
+    <tableColumn id="8" xr3:uid="{56059F27-4AC1-42B7-8136-8E16B7CD89F8}" name="BLKVOLUM"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium14" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -779,752 +779,752 @@
     </row>
     <row r="3" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A3" s="5">
-        <v>44022</v>
+        <v>44033</v>
       </c>
       <c r="B3">
-        <v>59.54</v>
+        <v>60.7</v>
       </c>
       <c r="C3">
-        <v>59.55</v>
+        <v>60.72</v>
       </c>
       <c r="D3">
-        <v>57.95</v>
+        <v>61.515000000000001</v>
       </c>
       <c r="E3">
-        <v>59.69</v>
+        <v>61.927500000000002</v>
       </c>
       <c r="F3">
-        <v>57.83</v>
+        <v>60.44</v>
       </c>
       <c r="G3">
-        <v>59.53</v>
+        <v>60.7</v>
       </c>
       <c r="H3">
-        <v>3095904</v>
+        <v>4746290</v>
       </c>
       <c r="N3" s="5">
-        <v>44022</v>
+        <v>44033</v>
       </c>
       <c r="O3">
-        <v>55.88</v>
+        <v>56.99</v>
       </c>
       <c r="P3">
-        <v>55.9</v>
+        <v>57</v>
       </c>
       <c r="Q3">
-        <v>57.54</v>
+        <v>57.805</v>
       </c>
       <c r="R3">
-        <v>58.15</v>
+        <v>58.5</v>
       </c>
       <c r="S3">
-        <v>55.51</v>
+        <v>56.317300000000003</v>
       </c>
       <c r="T3">
-        <v>55.88</v>
+        <v>57</v>
       </c>
       <c r="U3">
-        <v>3211604</v>
+        <v>2291926</v>
       </c>
     </row>
     <row r="4" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A4" s="5">
-        <v>44025</v>
+        <v>44034</v>
       </c>
       <c r="B4">
-        <v>58.57</v>
+        <v>61.03</v>
       </c>
       <c r="C4">
-        <v>58.59</v>
+        <v>61.04</v>
       </c>
       <c r="D4">
-        <v>59.84</v>
+        <v>61.31</v>
       </c>
       <c r="E4">
+        <v>61.765000000000001</v>
+      </c>
+      <c r="F4">
         <v>60.62</v>
       </c>
-      <c r="F4">
-        <v>58.39</v>
-      </c>
       <c r="G4">
-        <v>58.58</v>
+        <v>61.05</v>
       </c>
       <c r="H4">
-        <v>2783448</v>
+        <v>3947594</v>
       </c>
       <c r="N4" s="5">
-        <v>44025</v>
+        <v>44034</v>
       </c>
       <c r="O4">
-        <v>53.59</v>
+        <v>61.78</v>
       </c>
       <c r="P4">
-        <v>53.61</v>
+        <v>61.79</v>
       </c>
       <c r="Q4">
-        <v>56.68</v>
+        <v>57.07</v>
       </c>
       <c r="R4">
-        <v>58.35</v>
+        <v>62</v>
       </c>
       <c r="S4">
-        <v>53.38</v>
+        <v>56.97</v>
       </c>
       <c r="T4">
-        <v>53.59</v>
+        <v>61.79</v>
       </c>
       <c r="U4">
-        <v>3512482</v>
+        <v>6837200</v>
       </c>
     </row>
     <row r="5" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A5" s="5">
-        <v>44026</v>
+        <v>44035</v>
       </c>
       <c r="B5">
-        <v>58.95</v>
+        <v>60.48</v>
       </c>
       <c r="C5">
-        <v>58.96</v>
+        <v>60.51</v>
       </c>
       <c r="D5">
-        <v>57.8735</v>
+        <v>61.255000000000003</v>
       </c>
       <c r="E5">
-        <v>59.25</v>
+        <v>61.74</v>
       </c>
       <c r="F5">
-        <v>57.344999999999999</v>
+        <v>59.98</v>
       </c>
       <c r="G5">
-        <v>58.98</v>
+        <v>60.4</v>
       </c>
       <c r="H5">
-        <v>6630416</v>
+        <v>6101642</v>
       </c>
       <c r="N5" s="5">
-        <v>44026</v>
+        <v>44035</v>
       </c>
       <c r="O5">
-        <v>54.7</v>
+        <v>59.59</v>
       </c>
       <c r="P5">
-        <v>54.72</v>
+        <v>59.6</v>
       </c>
       <c r="Q5">
-        <v>53.3</v>
+        <v>61.63</v>
       </c>
       <c r="R5">
-        <v>54.86</v>
+        <v>62.33</v>
       </c>
       <c r="S5">
-        <v>52.26</v>
+        <v>58.6342</v>
       </c>
       <c r="T5">
-        <v>54.72</v>
+        <v>59.57</v>
       </c>
       <c r="U5">
-        <v>2781222</v>
+        <v>6591082</v>
       </c>
     </row>
     <row r="6" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A6" s="5">
-        <v>44027</v>
+        <v>44036</v>
       </c>
       <c r="B6">
-        <v>59.02</v>
+        <v>50.58</v>
       </c>
       <c r="C6">
-        <v>59.03</v>
+        <v>50.59</v>
       </c>
       <c r="D6">
-        <v>59.03</v>
+        <v>52.15</v>
       </c>
       <c r="E6">
-        <v>59.34</v>
+        <v>52.18</v>
       </c>
       <c r="F6">
-        <v>58.42</v>
+        <v>49.5</v>
       </c>
       <c r="G6">
-        <v>59.03</v>
+        <v>50.59</v>
       </c>
       <c r="H6">
-        <v>5529813</v>
+        <v>16019857</v>
       </c>
       <c r="N6" s="5">
-        <v>44027</v>
+        <v>44036</v>
       </c>
       <c r="O6">
-        <v>55.33</v>
+        <v>69.42</v>
       </c>
       <c r="P6">
-        <v>55.34</v>
+        <v>69.430000000000007</v>
       </c>
       <c r="Q6">
-        <v>54.96</v>
+        <v>64.180000000000007</v>
       </c>
       <c r="R6">
-        <v>55.37</v>
+        <v>69.94</v>
       </c>
       <c r="S6">
-        <v>53.59</v>
+        <v>64.05</v>
       </c>
       <c r="T6">
-        <v>55.34</v>
+        <v>69.400000000000006</v>
       </c>
       <c r="U6">
-        <v>3931487</v>
+        <v>11847972</v>
       </c>
     </row>
     <row r="7" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A7" s="5">
-        <v>44028</v>
+        <v>44039</v>
       </c>
       <c r="B7">
-        <v>59.14</v>
+        <v>49.56</v>
       </c>
       <c r="C7">
-        <v>59.15</v>
+        <v>49.57</v>
       </c>
       <c r="D7">
-        <v>58.54</v>
+        <v>51.03</v>
       </c>
       <c r="E7">
-        <v>59.36</v>
+        <v>51.14</v>
       </c>
       <c r="F7">
-        <v>58.4</v>
+        <v>49.465000000000003</v>
       </c>
       <c r="G7">
-        <v>59.14</v>
+        <v>49.57</v>
       </c>
       <c r="H7">
-        <v>1813790</v>
+        <v>39240052</v>
       </c>
       <c r="N7" s="5">
-        <v>44028</v>
+        <v>44039</v>
       </c>
       <c r="O7">
-        <v>54.91</v>
+        <v>68.959999999999994</v>
       </c>
       <c r="P7">
-        <v>54.92</v>
+        <v>68.98</v>
       </c>
       <c r="Q7">
-        <v>54.68</v>
+        <v>69.28</v>
       </c>
       <c r="R7">
-        <v>55.15</v>
+        <v>71.63</v>
       </c>
       <c r="S7">
-        <v>53.74</v>
+        <v>67.790000000000006</v>
       </c>
       <c r="T7">
-        <v>54.92</v>
+        <v>68.97</v>
       </c>
       <c r="U7">
-        <v>2785912</v>
+        <v>7895400</v>
       </c>
     </row>
     <row r="8" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A8" s="5">
-        <v>44029</v>
+        <v>44040</v>
       </c>
       <c r="B8">
-        <v>59.99</v>
+        <v>49.24</v>
       </c>
       <c r="C8">
-        <v>60</v>
+        <v>49.25</v>
       </c>
       <c r="D8">
-        <v>59.42</v>
+        <v>49.48</v>
       </c>
       <c r="E8">
-        <v>60.46</v>
+        <v>50.23</v>
       </c>
       <c r="F8">
-        <v>59.28</v>
+        <v>49.14</v>
       </c>
       <c r="G8">
-        <v>60</v>
+        <v>49.24</v>
       </c>
       <c r="H8">
-        <v>3465688</v>
+        <v>13759417</v>
       </c>
       <c r="N8" s="5">
-        <v>44029</v>
+        <v>44040</v>
       </c>
       <c r="O8">
-        <v>55.04</v>
+        <v>67.709999999999994</v>
       </c>
       <c r="P8">
-        <v>55.05</v>
+        <v>67.760000000000005</v>
       </c>
       <c r="Q8">
-        <v>55.31</v>
+        <v>68.099999999999994</v>
       </c>
       <c r="R8">
-        <v>55.81</v>
+        <v>69.8</v>
       </c>
       <c r="S8">
-        <v>54.68</v>
+        <v>67.02</v>
       </c>
       <c r="T8">
-        <v>55.04</v>
+        <v>67.61</v>
       </c>
       <c r="U8">
-        <v>3111670</v>
+        <v>4318006</v>
       </c>
     </row>
     <row r="9" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A9" s="5">
-        <v>44032</v>
+        <v>44041</v>
       </c>
       <c r="B9">
-        <v>61.14</v>
+        <v>48.07</v>
       </c>
       <c r="C9">
-        <v>61.15</v>
+        <v>48.08</v>
       </c>
       <c r="D9">
-        <v>60.08</v>
+        <v>49.49</v>
       </c>
       <c r="E9">
-        <v>61.38</v>
+        <v>49.5</v>
       </c>
       <c r="F9">
-        <v>59.34</v>
+        <v>47.9</v>
       </c>
       <c r="G9">
-        <v>61.15</v>
+        <v>48.07</v>
       </c>
       <c r="H9">
-        <v>3085279</v>
+        <v>6788006</v>
       </c>
       <c r="N9" s="5">
-        <v>44032</v>
+        <v>44041</v>
       </c>
       <c r="O9">
-        <v>57.45</v>
+        <v>76.09</v>
       </c>
       <c r="P9">
-        <v>57.46</v>
+        <v>76.099999999999994</v>
       </c>
       <c r="Q9">
-        <v>55.23</v>
+        <v>75.5</v>
       </c>
       <c r="R9">
-        <v>57.53</v>
+        <v>77.19</v>
       </c>
       <c r="S9">
-        <v>54.83</v>
+        <v>73.900000000000006</v>
       </c>
       <c r="T9">
-        <v>57.46</v>
+        <v>76.09</v>
       </c>
       <c r="U9">
-        <v>3018017</v>
+        <v>7342794</v>
       </c>
     </row>
     <row r="10" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A10" s="5">
-        <v>44033</v>
+        <v>44042</v>
       </c>
       <c r="B10">
-        <v>60.7</v>
+        <v>48</v>
       </c>
       <c r="C10">
-        <v>60.72</v>
+        <v>48.01</v>
       </c>
       <c r="D10">
-        <v>61.515000000000001</v>
+        <v>47.83</v>
       </c>
       <c r="E10">
-        <v>61.927500000000002</v>
+        <v>48.5</v>
       </c>
       <c r="F10">
-        <v>60.44</v>
+        <v>47.59</v>
       </c>
       <c r="G10">
-        <v>60.7</v>
+        <v>47.99</v>
       </c>
       <c r="H10">
-        <v>4746290</v>
+        <v>3884370</v>
       </c>
       <c r="N10" s="5">
-        <v>44033</v>
+        <v>44042</v>
       </c>
       <c r="O10">
-        <v>56.99</v>
+        <v>78.19</v>
       </c>
       <c r="P10">
-        <v>57</v>
+        <v>78.2</v>
       </c>
       <c r="Q10">
-        <v>57.805</v>
+        <v>75.37</v>
       </c>
       <c r="R10">
-        <v>58.5</v>
+        <v>78.959999999999994</v>
       </c>
       <c r="S10">
-        <v>56.317300000000003</v>
+        <v>75.069999999999993</v>
       </c>
       <c r="T10">
-        <v>57</v>
+        <v>78.2</v>
       </c>
       <c r="U10">
-        <v>2291926</v>
+        <v>3576867</v>
       </c>
     </row>
     <row r="11" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A11" s="5">
-        <v>44034</v>
+        <v>44043</v>
       </c>
       <c r="B11">
-        <v>61.03</v>
+        <v>47.73</v>
       </c>
       <c r="C11">
-        <v>61.04</v>
+        <v>47.74</v>
       </c>
       <c r="D11">
-        <v>61.31</v>
+        <v>48.13</v>
       </c>
       <c r="E11">
-        <v>61.765000000000001</v>
+        <v>48.321599999999997</v>
       </c>
       <c r="F11">
-        <v>60.62</v>
+        <v>46.97</v>
       </c>
       <c r="G11">
-        <v>61.05</v>
+        <v>47.73</v>
       </c>
       <c r="H11">
-        <v>3947594</v>
+        <v>10051456</v>
       </c>
       <c r="N11" s="5">
-        <v>44034</v>
+        <v>44043</v>
       </c>
       <c r="O11">
-        <v>61.78</v>
+        <v>77.42</v>
       </c>
       <c r="P11">
-        <v>61.79</v>
+        <v>77.430000000000007</v>
       </c>
       <c r="Q11">
-        <v>57.07</v>
+        <v>78.67</v>
       </c>
       <c r="R11">
-        <v>62</v>
+        <v>78.959999999999994</v>
       </c>
       <c r="S11">
-        <v>56.97</v>
+        <v>75.36</v>
       </c>
       <c r="T11">
-        <v>61.79</v>
+        <v>77.430000000000007</v>
       </c>
       <c r="U11">
-        <v>6837200</v>
+        <v>4718367</v>
       </c>
     </row>
     <row r="12" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A12" s="5">
-        <v>44035</v>
+        <v>44046</v>
       </c>
       <c r="B12">
-        <v>60.48</v>
+        <v>48.28</v>
       </c>
       <c r="C12">
-        <v>60.51</v>
+        <v>48.29</v>
       </c>
       <c r="D12">
-        <v>61.255000000000003</v>
+        <v>48.27</v>
       </c>
       <c r="E12">
-        <v>61.74</v>
+        <v>48.6267</v>
       </c>
       <c r="F12">
-        <v>59.98</v>
+        <v>47.74</v>
       </c>
       <c r="G12">
-        <v>60.4</v>
+        <v>48.3</v>
       </c>
       <c r="H12">
-        <v>6101642</v>
+        <v>5617516</v>
       </c>
       <c r="N12" s="5">
-        <v>44035</v>
+        <v>44046</v>
       </c>
       <c r="O12">
-        <v>59.59</v>
+        <v>77.650000000000006</v>
       </c>
       <c r="P12">
-        <v>59.6</v>
+        <v>77.66</v>
       </c>
       <c r="Q12">
-        <v>61.63</v>
+        <v>78.19</v>
       </c>
       <c r="R12">
-        <v>62.33</v>
+        <v>78.5</v>
       </c>
       <c r="S12">
-        <v>58.6342</v>
+        <v>77.06</v>
       </c>
       <c r="T12">
-        <v>59.57</v>
+        <v>77.67</v>
       </c>
       <c r="U12">
-        <v>6591082</v>
+        <v>2743098</v>
       </c>
     </row>
     <row r="13" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A13" s="5">
-        <v>44036</v>
+        <v>44047</v>
       </c>
       <c r="B13">
-        <v>50.58</v>
+        <v>49.13</v>
       </c>
       <c r="C13">
-        <v>50.59</v>
+        <v>49.14</v>
       </c>
       <c r="D13">
-        <v>52.15</v>
+        <v>48.6</v>
       </c>
       <c r="E13">
-        <v>52.18</v>
+        <v>49.14</v>
       </c>
       <c r="F13">
-        <v>49.5</v>
+        <v>48.5</v>
       </c>
       <c r="G13">
-        <v>50.59</v>
+        <v>49.13</v>
       </c>
       <c r="H13">
-        <v>16019857</v>
+        <v>4870512</v>
       </c>
       <c r="N13" s="5">
-        <v>44036</v>
+        <v>44047</v>
       </c>
       <c r="O13">
-        <v>69.42</v>
+        <v>85.04</v>
       </c>
       <c r="P13">
-        <v>69.430000000000007</v>
+        <v>85.05</v>
       </c>
       <c r="Q13">
-        <v>64.180000000000007</v>
+        <v>78.03</v>
       </c>
       <c r="R13">
-        <v>69.94</v>
+        <v>85.805000000000007</v>
       </c>
       <c r="S13">
-        <v>64.05</v>
+        <v>77.989999999999995</v>
       </c>
       <c r="T13">
-        <v>69.400000000000006</v>
+        <v>85.04</v>
       </c>
       <c r="U13">
-        <v>11847972</v>
+        <v>9498960</v>
       </c>
     </row>
     <row r="14" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A14" s="5">
-        <v>44039</v>
+        <v>44048</v>
       </c>
       <c r="B14">
-        <v>49.56</v>
+        <v>48.92</v>
       </c>
       <c r="C14">
-        <v>49.57</v>
+        <v>48.93</v>
       </c>
       <c r="D14">
-        <v>51.03</v>
+        <v>49.72</v>
       </c>
       <c r="E14">
-        <v>51.14</v>
+        <v>49.72</v>
       </c>
       <c r="F14">
-        <v>49.465000000000003</v>
+        <v>48.66</v>
       </c>
       <c r="G14">
-        <v>49.57</v>
+        <v>48.92</v>
       </c>
       <c r="H14">
-        <v>39240052</v>
+        <v>6427933</v>
       </c>
       <c r="N14" s="5">
-        <v>44039</v>
+        <v>44048</v>
       </c>
       <c r="O14">
-        <v>68.959999999999994</v>
+        <v>85.31</v>
       </c>
       <c r="P14">
-        <v>68.98</v>
+        <v>85.33</v>
       </c>
       <c r="Q14">
-        <v>69.28</v>
+        <v>84.96</v>
       </c>
       <c r="R14">
-        <v>71.63</v>
+        <v>86.32</v>
       </c>
       <c r="S14">
-        <v>67.790000000000006</v>
+        <v>83.32</v>
       </c>
       <c r="T14">
-        <v>68.97</v>
+        <v>85.31</v>
       </c>
       <c r="U14">
-        <v>7895400</v>
+        <v>2882107</v>
       </c>
     </row>
     <row r="15" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A15" s="5">
-        <v>44040</v>
+        <v>44049</v>
       </c>
       <c r="B15">
-        <v>49.24</v>
+        <v>48.57</v>
       </c>
       <c r="C15">
-        <v>49.25</v>
+        <v>48.58</v>
       </c>
       <c r="D15">
-        <v>49.48</v>
+        <v>48.79</v>
       </c>
       <c r="E15">
-        <v>50.23</v>
+        <v>48.82</v>
       </c>
       <c r="F15">
-        <v>49.14</v>
+        <v>48.1</v>
       </c>
       <c r="G15">
-        <v>49.24</v>
+        <v>48.57</v>
       </c>
       <c r="H15">
-        <v>13759417</v>
+        <v>4123124</v>
       </c>
       <c r="N15" s="5">
-        <v>44040</v>
+        <v>44049</v>
       </c>
       <c r="O15">
-        <v>67.709999999999994</v>
+        <v>86.7</v>
       </c>
       <c r="P15">
-        <v>67.760000000000005</v>
+        <v>86.72</v>
       </c>
       <c r="Q15">
-        <v>68.099999999999994</v>
+        <v>85.49</v>
       </c>
       <c r="R15">
-        <v>69.8</v>
+        <v>86.98</v>
       </c>
       <c r="S15">
-        <v>67.02</v>
+        <v>84.780100000000004</v>
       </c>
       <c r="T15">
-        <v>67.61</v>
+        <v>86.71</v>
       </c>
       <c r="U15">
-        <v>4318006</v>
+        <v>2350458</v>
       </c>
     </row>
     <row r="16" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A16" s="5">
-        <v>44041</v>
+        <v>44050</v>
       </c>
       <c r="B16">
-        <v>48.07</v>
+        <v>48.03</v>
       </c>
       <c r="C16">
-        <v>48.08</v>
+        <v>48.04</v>
       </c>
       <c r="D16">
-        <v>49.49</v>
+        <v>48.53</v>
       </c>
       <c r="E16">
-        <v>49.5</v>
+        <v>48.65</v>
       </c>
       <c r="F16">
-        <v>47.9</v>
+        <v>47.7</v>
       </c>
       <c r="G16">
-        <v>48.07</v>
+        <v>48.03</v>
       </c>
       <c r="H16">
-        <v>6788006</v>
+        <v>12055972</v>
       </c>
       <c r="N16" s="5">
-        <v>44041</v>
+        <v>44050</v>
       </c>
       <c r="O16">
-        <v>76.09</v>
+        <v>84.82</v>
       </c>
       <c r="P16">
-        <v>76.099999999999994</v>
+        <v>84.85</v>
       </c>
       <c r="Q16">
-        <v>75.5</v>
+        <v>86.67</v>
       </c>
       <c r="R16">
-        <v>77.19</v>
+        <v>87.29</v>
       </c>
       <c r="S16">
-        <v>73.900000000000006</v>
+        <v>82.670199999999994</v>
       </c>
       <c r="T16">
-        <v>76.09</v>
+        <v>84.85</v>
       </c>
       <c r="U16">
-        <v>7342794</v>
+        <v>2902196</v>
       </c>
     </row>
     <row r="17" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A17" s="5">
-        <v>44042</v>
+        <v>44053</v>
       </c>
       <c r="B17">
-        <v>48</v>
+        <v>49.22</v>
       </c>
       <c r="C17">
-        <v>48.01</v>
+        <v>49.23</v>
       </c>
       <c r="D17">
-        <v>47.83</v>
+        <v>48.2</v>
       </c>
       <c r="E17">
-        <v>48.5</v>
+        <v>49.39</v>
       </c>
       <c r="F17">
-        <v>47.59</v>
+        <v>48.06</v>
       </c>
       <c r="G17">
-        <v>47.99</v>
+        <v>49.22</v>
       </c>
       <c r="H17">
-        <v>3884370</v>
+        <v>13730994</v>
       </c>
       <c r="N17" s="5">
-        <v>44042</v>
+        <v>44053</v>
       </c>
       <c r="O17">
-        <v>78.19</v>
+        <v>82.23</v>
       </c>
       <c r="P17">
-        <v>78.2</v>
+        <v>82.24</v>
       </c>
       <c r="Q17">
-        <v>75.37</v>
+        <v>85.05</v>
       </c>
       <c r="R17">
-        <v>78.959999999999994</v>
+        <v>85.16</v>
       </c>
       <c r="S17">
-        <v>75.069999999999993</v>
+        <v>79.322100000000006</v>
       </c>
       <c r="T17">
-        <v>78.2</v>
+        <v>82.24</v>
       </c>
       <c r="U17">
-        <v>3576867</v>
+        <v>3337267</v>
       </c>
     </row>
     <row r="24" spans="1:21" x14ac:dyDescent="0.25">

</xml_diff>